<commit_message>
Added AL Project to List
</commit_message>
<xml_diff>
--- a/Game List.xlsx
+++ b/Game List.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Emulators\ArcadeSafety\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jorda\Documents\UCF Arcade\ArcadeSafetyGit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4C99D6C-AD5C-4DDE-9426-2AB1553ACAA1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CADB6A2B-EC9D-44E0-8E7E-49E1CBE66AFD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="5865" xr2:uid="{87FE2530-ACA9-4CC4-87DD-CA7614213A2F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{87FE2530-ACA9-4CC4-87DD-CA7614213A2F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,6 +23,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
   <si>
     <t>Balloon Burst</t>
   </si>
@@ -159,6 +160,9 @@
   </si>
   <si>
     <t>ToxicMonstersArcade</t>
+  </si>
+  <si>
+    <t>arcadeLightController</t>
   </si>
 </sst>
 </file>
@@ -517,10 +521,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5C52D14-62FD-4548-B51D-713A41BE5310}">
-  <dimension ref="A1:C41"/>
+  <dimension ref="A1:C42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A41"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -532,382 +536,391 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="str">
-        <f t="shared" ref="A1:A41" ca="1" si="0">"G"&amp;ROW()-1&amp;"="""&amp;INDIRECT("B" &amp; ROW())&amp;".exe"""</f>
-        <v>G0="AD5.exe"</v>
+        <f ca="1">"G"&amp;ROW()-1&amp;"="""&amp;INDIRECT("B" &amp; ROW())&amp;".exe"""</f>
+        <v>G0="arcadeLightController.exe"</v>
       </c>
       <c r="B1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C1" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>G1="AGHR_SVAD.exe"</v>
+        <f ca="1">"G"&amp;ROW()-1&amp;"="""&amp;INDIRECT("B" &amp; ROW())&amp;".exe"""</f>
+        <v>G1="AD5.exe"</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>G2="Balloon Burst.exe"</v>
+        <f t="shared" ref="A3:A42" ca="1" si="0">"G"&amp;ROW()-1&amp;"="""&amp;INDIRECT("B" &amp; ROW())&amp;".exe"""</f>
+        <v>G2="AGHR_SVAD.exe"</v>
       </c>
       <c r="B3" t="s">
-        <v>0</v>
+        <v>9</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>G3="BattleBuddies.exe"</v>
+        <v>G3="Balloon Burst.exe"</v>
       </c>
       <c r="B4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>G4="BossRun_Arcade.exe"</v>
+        <v>G4="BattleBuddies.exe"</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>G5="Bounty Breaker Arcade.exe"</v>
+        <v>G5="BossRun_Arcade.exe"</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>G6="ChannelCruisersArcade.exe"</v>
+        <v>G6="Bounty Breaker Arcade.exe"</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>G7="Child's Play.exe"</v>
+        <v>G7="ChannelCruisersArcade.exe"</v>
       </c>
       <c r="B8" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>G8="Dusk_PC_Build.exe"</v>
+        <v>G8="Child's Play.exe"</v>
       </c>
       <c r="B9" t="s">
-        <v>13</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>G9="FFRR_Arcade.exe"</v>
+        <v>G9="Dusk_PC_Build.exe"</v>
       </c>
       <c r="B10" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>G10="Fish Frenzy Arcade.exe"</v>
+        <v>G10="FFRR_Arcade.exe"</v>
       </c>
       <c r="B11" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>G11="JamBall_3Fix.exe"</v>
+        <v>G11="Fish Frenzy Arcade.exe"</v>
       </c>
       <c r="B12" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>G12="Knockout Knights - Arcade.exe"</v>
+        <v>G12="JamBall_3Fix.exe"</v>
       </c>
       <c r="B13" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>G13="KrakenSkulls.exe"</v>
+        <v>G13="Knockout Knights - Arcade.exe"</v>
       </c>
       <c r="B14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>G14="LlamasRevenge.exe"</v>
+        <v>G14="KrakenSkulls.exe"</v>
       </c>
       <c r="B15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>G15="M3_Arcade.exe"</v>
+        <v>G15="LlamasRevenge.exe"</v>
       </c>
       <c r="B16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>G16="M-GPX Dashers.exe"</v>
+        <v>G16="M3_Arcade.exe"</v>
       </c>
       <c r="B17" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>G17="MonocleMatchDungeonArcade.exe"</v>
+        <v>G17="M-GPX Dashers.exe"</v>
       </c>
       <c r="B18" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>G18="NeonKnights.exe"</v>
+        <v>G18="MonocleMatchDungeonArcade.exe"</v>
       </c>
       <c r="B19" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>G19="NightMare.exe"</v>
+        <v>G19="NeonKnights.exe"</v>
       </c>
       <c r="B20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>G20="Occupation Big.exe"</v>
+        <v>G20="NightMare.exe"</v>
       </c>
       <c r="B21" t="s">
-        <v>3</v>
+        <v>33</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>G21="Outerlaw.exe"</v>
+        <v>G21="Occupation Big.exe"</v>
       </c>
       <c r="B22" t="s">
-        <v>34</v>
+        <v>3</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>G22="PDF_arcade.exe"</v>
+        <v>G22="Outerlaw.exe"</v>
       </c>
       <c r="B23" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>G23="PhaseJumper_Arcade.exe"</v>
+        <v>G23="PDF_arcade.exe"</v>
       </c>
       <c r="B24" t="s">
-        <v>15</v>
+        <v>35</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>G24="PowerDefenderBuild_Arcade.exe"</v>
+        <v>G24="PhaseJumper_Arcade.exe"</v>
       </c>
       <c r="B25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>G25="PPP.exe"</v>
+        <v>G25="PowerDefenderBuild_Arcade.exe"</v>
       </c>
       <c r="B26" t="s">
-        <v>36</v>
+        <v>16</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>G26="RhythmRumbleArcade.exe"</v>
+        <v>G26="PPP.exe"</v>
       </c>
       <c r="B27" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>G27="ROCKETTRON.exe"</v>
+        <v>G27="RhythmRumbleArcade.exe"</v>
       </c>
       <c r="B28" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>G28="RR_Arcade_FinalBuild_Arcade.exe"</v>
+        <v>G28="ROCKETTRON.exe"</v>
       </c>
       <c r="B29" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>G29="SA Build.exe"</v>
+        <v>G29="RR_Arcade_FinalBuild_Arcade.exe"</v>
       </c>
       <c r="B30" t="s">
-        <v>17</v>
+        <v>38</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>G30="SafehavenFinalArcade.exe"</v>
+        <v>G30="SA Build.exe"</v>
       </c>
       <c r="B31" t="s">
-        <v>40</v>
+        <v>17</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>G31="SkyscrappersArcadeFixedIPromiseThisTimeEdition.exe"</v>
+        <v>G31="SafehavenFinalArcade.exe"</v>
       </c>
       <c r="B32" t="s">
-        <v>18</v>
+        <v>40</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>G32="Slayzers.exe"</v>
+        <v>G32="SkyscrappersArcadeFixedIPromiseThisTimeEdition.exe"</v>
       </c>
       <c r="B33" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>G33="slowdown.exe"</v>
+        <v>G33="Slayzers.exe"</v>
       </c>
       <c r="B34" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>G34="StarPower.exe"</v>
+        <v>G34="slowdown.exe"</v>
       </c>
       <c r="B35" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>G35="SuperSonicJetPacks_ArcadeBuild.exe"</v>
+        <v>G35="StarPower.exe"</v>
       </c>
       <c r="B36" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>G36="SUSHI_SLAP_ARCADE.exe"</v>
+        <v>G36="SuperSonicJetPacks_ArcadeBuild.exe"</v>
       </c>
       <c r="B37" t="s">
-        <v>41</v>
+        <v>20</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>G37="Time_Tilt_Arcade.exe"</v>
+        <v>G37="SUSHI_SLAP_ARCADE.exe"</v>
       </c>
       <c r="B38" t="s">
-        <v>21</v>
+        <v>41</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>G38="ToxicMonstersArcade.exe"</v>
+        <v>G38="Time_Tilt_Arcade.exe"</v>
       </c>
       <c r="B39" t="s">
-        <v>42</v>
+        <v>21</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>G39="Unreel_Fishing_Arcade_Edition.exe"</v>
+        <v>G39="ToxicMonstersArcade.exe"</v>
       </c>
       <c r="B40" t="s">
-        <v>22</v>
+        <v>42</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>G40="ValkFinalBuild.exe"</v>
+        <v>G40="Unreel_Fishing_Arcade_Edition.exe"</v>
       </c>
       <c r="B41" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>G41="ValkFinalBuild.exe"</v>
+      </c>
+      <c r="B42" t="s">
         <v>23</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:C46">
-    <sortCondition ref="B1"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:C47">
+    <sortCondition ref="B2"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>